<commit_message>
new genres import and order
</commit_message>
<xml_diff>
--- a/data/genres.xlsx
+++ b/data/genres.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="346">
   <si>
     <t>Alternative</t>
   </si>
@@ -132,7 +132,7 @@
     <t>Chanukah</t>
   </si>
   <si>
-    <t>CCM</t>
+    <t>Ccm</t>
   </si>
   <si>
     <t>J-Rock</t>
@@ -144,7 +144,7 @@
     <t>Alternativo &amp; Rock Latino</t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative metal </t>
+    <t xml:space="preserve">Alternative Metal </t>
   </si>
   <si>
     <t>Environmental</t>
@@ -171,7 +171,7 @@
     <t>Chicano</t>
   </si>
   <si>
-    <t xml:space="preserve">A cappella </t>
+    <t xml:space="preserve">A Cappella </t>
   </si>
   <si>
     <t>Alternative Rock</t>
@@ -189,7 +189,7 @@
     <t>Standup Comedy</t>
   </si>
   <si>
-    <t>TV Themes</t>
+    <t>Tv Themes</t>
   </si>
   <si>
     <t>Americana</t>
@@ -219,10 +219,10 @@
     <t>Avant-Garde Jazz</t>
   </si>
   <si>
-    <t>Argentine tango</t>
-  </si>
-  <si>
-    <t>Avant-garde metal</t>
+    <t>Argentine Tango</t>
+  </si>
+  <si>
+    <t>Avant-Garde Metal</t>
   </si>
   <si>
     <t>Healing</t>
@@ -294,10 +294,10 @@
     <t xml:space="preserve">Bebop </t>
   </si>
   <si>
-    <t>Baladas y Boleros</t>
-  </si>
-  <si>
-    <t>Bay Area thrash metal</t>
+    <t>Baladas Y Boleros</t>
+  </si>
+  <si>
+    <t>Bay Area Thrash Metal</t>
   </si>
   <si>
     <t>Meditation</t>
@@ -324,7 +324,7 @@
     <t>Conjunto</t>
   </si>
   <si>
-    <t xml:space="preserve">Doo-wop </t>
+    <t xml:space="preserve">Doo-Wop </t>
   </si>
   <si>
     <t>Experimental Rock</t>
@@ -366,7 +366,7 @@
     <t xml:space="preserve">Bossa Nova </t>
   </si>
   <si>
-    <t xml:space="preserve">Black metal </t>
+    <t xml:space="preserve">Black Metal </t>
   </si>
   <si>
     <t>Nature</t>
@@ -426,7 +426,7 @@
     <t>Brazilian</t>
   </si>
   <si>
-    <t xml:space="preserve">Blackened death metal </t>
+    <t xml:space="preserve">Blackened Death Metal </t>
   </si>
   <si>
     <t>Relaxation</t>
@@ -444,7 +444,7 @@
     <t>Folk-Roc</t>
   </si>
   <si>
-    <t>TV Soundtrack</t>
+    <t>Tv Soundtrack</t>
   </si>
   <si>
     <t>New Mex</t>
@@ -543,7 +543,7 @@
     <t xml:space="preserve">Flamenco </t>
   </si>
   <si>
-    <t>Celtic metal</t>
+    <t>Celtic Metal</t>
   </si>
   <si>
     <t>Electro Pop</t>
@@ -591,7 +591,7 @@
     <t>Latin Jazz</t>
   </si>
   <si>
-    <t xml:space="preserve">Christian metal </t>
+    <t xml:space="preserve">Christian Metal </t>
   </si>
   <si>
     <t>Indie Pop</t>
@@ -621,7 +621,7 @@
     <t xml:space="preserve">Glitch Hop </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro-swing </t>
+    <t xml:space="preserve">Electro-Swing </t>
   </si>
   <si>
     <t>Old School Rap</t>
@@ -639,7 +639,7 @@
     <t xml:space="preserve">Nuevo Flamenco </t>
   </si>
   <si>
-    <t>Crossover thrash</t>
+    <t>Crossover Thrash</t>
   </si>
   <si>
     <t>Orchestral Pop</t>
@@ -651,7 +651,7 @@
     <t>Art Rock</t>
   </si>
   <si>
-    <t xml:space="preserve">Lo-fi </t>
+    <t xml:space="preserve">Lo-Fi </t>
   </si>
   <si>
     <t>Medieval</t>
@@ -675,13 +675,13 @@
     <t>Praise &amp; Worship</t>
   </si>
   <si>
-    <t>Ethio-jazz (with thx to Jillian Edwards)</t>
+    <t>Ethio-Jazz (with Thx To Jillian Edwards)</t>
   </si>
   <si>
     <t>Pop Latino</t>
   </si>
   <si>
-    <t>Cyber metal</t>
+    <t>Cyber Metal</t>
   </si>
   <si>
     <t>Pop/Rock</t>
@@ -714,16 +714,16 @@
     <t>Christmas: Rock</t>
   </si>
   <si>
-    <t>Qawwali (with thx to Jillian Edwards)</t>
+    <t>Qawwali (with Thx To Jillian Edwards)</t>
   </si>
   <si>
     <t>Fusion</t>
   </si>
   <si>
-    <t xml:space="preserve">Portuguese fado </t>
-  </si>
-  <si>
-    <t>Dark metal</t>
+    <t xml:space="preserve">Portuguese Fado </t>
+  </si>
+  <si>
+    <t>Dark Metal</t>
   </si>
   <si>
     <t xml:space="preserve">Power Pop </t>
@@ -744,7 +744,7 @@
     <t>Urban Cowboy</t>
   </si>
   <si>
-    <t>Hi-NRG / Eurodance</t>
+    <t>Hi-Nrg / Eurodance</t>
   </si>
   <si>
     <t xml:space="preserve">Hardstyle </t>
@@ -759,13 +759,13 @@
     <t>Southern Gospel</t>
   </si>
   <si>
-    <t>Gypsy Jazz (kudos to Mike Tait Tafoya)</t>
+    <t>Gypsy Jazz (kudos To Mike Tait Tafoya)</t>
   </si>
   <si>
     <t>Raíces</t>
   </si>
   <si>
-    <t xml:space="preserve">Death metal </t>
+    <t xml:space="preserve">Death Metal </t>
   </si>
   <si>
     <t>Soft Rock</t>
@@ -786,7 +786,7 @@
     <t>House</t>
   </si>
   <si>
-    <t>IDM/Experimental</t>
+    <t>Idm/Experimental</t>
   </si>
   <si>
     <t>West Coast Rap</t>
@@ -801,10 +801,10 @@
     <t>Hard Bop</t>
   </si>
   <si>
-    <t>Reggaeton y Hip-Hop</t>
-  </si>
-  <si>
-    <t>Death 'n' roll</t>
+    <t>Reggaeton Y Hip-Hop</t>
+  </si>
+  <si>
+    <t>Death 'n' Roll</t>
   </si>
   <si>
     <t>Synthpop</t>
@@ -861,10 +861,10 @@
     <t>Mainstream Jazz</t>
   </si>
   <si>
-    <t>Salsa y Tropical</t>
-  </si>
-  <si>
-    <t>Digital hardcore</t>
+    <t>Salsa Y Tropical</t>
+  </si>
+  <si>
+    <t>Digital Hardcore</t>
   </si>
   <si>
     <t>Hair Metal</t>
@@ -891,7 +891,7 @@
     <t>Smooth Jazz</t>
   </si>
   <si>
-    <t xml:space="preserve">Doom metal </t>
+    <t xml:space="preserve">Doom Metal </t>
   </si>
   <si>
     <t>Trance</t>
@@ -900,7 +900,7 @@
     <t>Trad Jazz</t>
   </si>
   <si>
-    <t>Drone metal</t>
+    <t>Drone Metal</t>
   </si>
   <si>
     <t>Industrial Rock</t>
@@ -915,22 +915,22 @@
     <t>Jam Bands</t>
   </si>
   <si>
-    <t xml:space="preserve">Extreme metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folk metal </t>
+    <t xml:space="preserve">Extreme Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folk Metal </t>
   </si>
   <si>
     <t>Noise Rock</t>
   </si>
   <si>
-    <t xml:space="preserve">Funk metal </t>
+    <t xml:space="preserve">Funk Metal </t>
   </si>
   <si>
     <t xml:space="preserve">Post Punk </t>
   </si>
   <si>
-    <t xml:space="preserve">Glam metal </t>
+    <t xml:space="preserve">Glam Metal </t>
   </si>
   <si>
     <t>Prog-Rock/Art Rock</t>
@@ -942,9 +942,6 @@
     <t>Psychedelic</t>
   </si>
   <si>
-    <t xml:space="preserve">Gothic metal </t>
-  </si>
-  <si>
     <t>Rock &amp; Roll</t>
   </si>
   <si>
@@ -954,34 +951,34 @@
     <t xml:space="preserve">Rockabilly </t>
   </si>
   <si>
-    <t xml:space="preserve">Groove metal </t>
+    <t xml:space="preserve">Groove Metal </t>
   </si>
   <si>
     <t>Roots Rock</t>
   </si>
   <si>
-    <t xml:space="preserve">Industrial metal </t>
-  </si>
-  <si>
-    <t>Latin metal</t>
+    <t xml:space="preserve">Industrial Metal </t>
+  </si>
+  <si>
+    <t>Latin Metal</t>
   </si>
   <si>
     <t>Southern Rock</t>
   </si>
   <si>
-    <t>Medieval metal</t>
+    <t>Medieval Metal</t>
   </si>
   <si>
     <t>Space Rock</t>
   </si>
   <si>
-    <t xml:space="preserve">Melodic death metal </t>
+    <t xml:space="preserve">Melodic Death Metal </t>
   </si>
   <si>
     <t>Surf</t>
   </si>
   <si>
-    <t>Melodic metalcore</t>
+    <t>Melodic Metalcore</t>
   </si>
   <si>
     <t>Metalcore</t>
@@ -990,10 +987,10 @@
     <t>Time Lord Rock</t>
   </si>
   <si>
-    <t>Nagoya kei</t>
-  </si>
-  <si>
-    <t>Neoclassical metal</t>
+    <t>Nagoya Kei</t>
+  </si>
+  <si>
+    <t>Neoclassical Metal</t>
   </si>
   <si>
     <t>Neue Deutsche Härte</t>
@@ -1002,58 +999,58 @@
     <t xml:space="preserve">Nintendocore </t>
   </si>
   <si>
-    <t xml:space="preserve">Nu metal </t>
-  </si>
-  <si>
-    <t>Pagan metal</t>
-  </si>
-  <si>
-    <t>Pirate metal</t>
+    <t xml:space="preserve">Nu Metal </t>
+  </si>
+  <si>
+    <t>Pagan Metal</t>
+  </si>
+  <si>
+    <t>Pirate Metal</t>
   </si>
   <si>
     <t>Pornogrind</t>
   </si>
   <si>
-    <t xml:space="preserve">Post-metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progressive metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rap metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sludge metal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed metal </t>
-  </si>
-  <si>
-    <t>Stoner rock</t>
-  </si>
-  <si>
-    <t>Symphonic black metal</t>
-  </si>
-  <si>
-    <t>Symphonic metal</t>
-  </si>
-  <si>
-    <t>Thrash metal</t>
-  </si>
-  <si>
-    <t>Heavy metal</t>
-  </si>
-  <si>
-    <t>Unblack metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viking metal </t>
-  </si>
-  <si>
-    <t>Visual kei</t>
+    <t xml:space="preserve">Post-Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progressive Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rap Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sludge Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed Metal </t>
+  </si>
+  <si>
+    <t>Stoner Rock</t>
+  </si>
+  <si>
+    <t>Symphonic Black Metal</t>
+  </si>
+  <si>
+    <t>Symphonic Metal</t>
+  </si>
+  <si>
+    <t>Thrash Metal</t>
+  </si>
+  <si>
+    <t>Heavy Metal</t>
+  </si>
+  <si>
+    <t>Unblack Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viking Metal </t>
+  </si>
+  <si>
+    <t>Visual Kei</t>
   </si>
 </sst>
 </file>
@@ -1063,11 +1060,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1075,7 +1072,12 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -1123,23 +1125,20 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1170,9 +1169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office Theme">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -1210,7 +1209,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office Theme">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Helvetica"/>
         <a:ea typeface="Helvetica"/>
@@ -1222,7 +1221,7 @@
         <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office Theme">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1295,22 +1294,10 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
@@ -1387,16 +1374,10 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1415,7 +1396,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1424,10 +1405,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1973,7 +1954,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1992,7 +1973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2001,10 +1982,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2259,37 +2240,37 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1719" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1719" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6797" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.6094" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.0703" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85156" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.6719" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="26" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1719" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.67188" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.67188" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.67188" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.3516" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.67188" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.8516" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.6719" style="1" customWidth="1"/>
+    <col min="18" max="18" width="26.1719" style="1" customWidth="1"/>
     <col min="19" max="19" width="19.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85156" style="1" customWidth="1"/>
-    <col min="22" max="22" width="8.85156" style="1" customWidth="1"/>
-    <col min="23" max="23" width="22.6719" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6719" style="1" customWidth="1"/>
-    <col min="25" max="25" width="8.85156" style="1" customWidth="1"/>
-    <col min="26" max="26" width="8.85156" style="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85156" style="1" customWidth="1"/>
-    <col min="28" max="28" width="8.85156" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85156" style="1" customWidth="1"/>
+    <col min="20" max="20" width="29.6719" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.67188" style="1" customWidth="1"/>
+    <col min="22" max="22" width="8.67188" style="1" customWidth="1"/>
+    <col min="23" max="23" width="22.8516" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.8516" style="1" customWidth="1"/>
+    <col min="25" max="25" width="8.67188" style="1" customWidth="1"/>
+    <col min="26" max="26" width="8.67188" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.67188" style="1" customWidth="1"/>
+    <col min="28" max="28" width="8.67188" style="1" customWidth="1"/>
+    <col min="29" max="29" width="8.67188" style="1" customWidth="1"/>
     <col min="30" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2378,7 +2359,7 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
+    <row r="2" ht="13.65" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3746,14 +3727,14 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" t="s" s="2">
-        <v>309</v>
+        <v>275</v>
       </c>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
@@ -3781,14 +3762,14 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
@@ -3816,14 +3797,14 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
@@ -3851,7 +3832,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -3886,14 +3867,14 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
@@ -3921,14 +3902,14 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="W32" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
@@ -3956,14 +3937,14 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
@@ -3991,7 +3972,7 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -4026,14 +4007,14 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
       <c r="W35" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
@@ -4061,7 +4042,7 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -4094,7 +4075,7 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -4127,7 +4108,7 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -4160,7 +4141,7 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
       <c r="R39" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -4193,7 +4174,7 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
@@ -4226,7 +4207,7 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
@@ -4259,7 +4240,7 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -4292,7 +4273,7 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
@@ -4325,7 +4306,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -4358,7 +4339,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
       <c r="R45" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
@@ -4391,7 +4372,7 @@
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
@@ -4424,7 +4405,7 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
       <c r="R47" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
@@ -4457,7 +4438,7 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
@@ -4490,7 +4471,7 @@
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
       <c r="R49" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
@@ -4523,7 +4504,7 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -4556,7 +4537,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
@@ -4589,7 +4570,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
@@ -4622,7 +4603,7 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
@@ -4655,7 +4636,7 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
@@ -4688,7 +4669,7 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
@@ -4721,7 +4702,7 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
@@ -4754,7 +4735,7 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
@@ -4768,7 +4749,7 @@
       <c r="AB57" s="3"/>
       <c r="AC57" s="3"/>
     </row>
-    <row r="58" ht="15" customHeight="1">
+    <row r="58" ht="13.65" customHeight="1">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4799,7 +4780,7 @@
       <c r="AB58" s="3"/>
       <c r="AC58" s="3"/>
     </row>
-    <row r="59" ht="15" customHeight="1">
+    <row r="59" ht="13.65" customHeight="1">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4830,7 +4811,7 @@
       <c r="AB59" s="3"/>
       <c r="AC59" s="3"/>
     </row>
-    <row r="60" ht="15" customHeight="1">
+    <row r="60" ht="13.65" customHeight="1">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4861,7 +4842,7 @@
       <c r="AB60" s="3"/>
       <c r="AC60" s="3"/>
     </row>
-    <row r="61" ht="15" customHeight="1">
+    <row r="61" ht="13.65" customHeight="1">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4892,7 +4873,7 @@
       <c r="AB61" s="3"/>
       <c r="AC61" s="3"/>
     </row>
-    <row r="62" ht="15" customHeight="1">
+    <row r="62" ht="13.65" customHeight="1">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4923,7 +4904,7 @@
       <c r="AB62" s="3"/>
       <c r="AC62" s="3"/>
     </row>
-    <row r="63" ht="15" customHeight="1">
+    <row r="63" ht="13.65" customHeight="1">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4954,7 +4935,7 @@
       <c r="AB63" s="3"/>
       <c r="AC63" s="3"/>
     </row>
-    <row r="64" ht="15" customHeight="1">
+    <row r="64" ht="13.65" customHeight="1">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4985,7 +4966,7 @@
       <c r="AB64" s="3"/>
       <c r="AC64" s="3"/>
     </row>
-    <row r="65" ht="15" customHeight="1">
+    <row r="65" ht="13.65" customHeight="1">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -5016,7 +4997,7 @@
       <c r="AB65" s="3"/>
       <c r="AC65" s="3"/>
     </row>
-    <row r="66" ht="15" customHeight="1">
+    <row r="66" ht="13.65" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -5047,7 +5028,7 @@
       <c r="AB66" s="3"/>
       <c r="AC66" s="3"/>
     </row>
-    <row r="67" ht="15" customHeight="1">
+    <row r="67" ht="13.65" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -5078,7 +5059,7 @@
       <c r="AB67" s="3"/>
       <c r="AC67" s="3"/>
     </row>
-    <row r="68" ht="15" customHeight="1">
+    <row r="68" ht="13.65" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -5109,7 +5090,7 @@
       <c r="AB68" s="3"/>
       <c r="AC68" s="3"/>
     </row>
-    <row r="69" ht="15" customHeight="1">
+    <row r="69" ht="13.65" customHeight="1">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -5140,7 +5121,7 @@
       <c r="AB69" s="3"/>
       <c r="AC69" s="3"/>
     </row>
-    <row r="70" ht="15" customHeight="1">
+    <row r="70" ht="13.65" customHeight="1">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -5171,7 +5152,7 @@
       <c r="AB70" s="3"/>
       <c r="AC70" s="3"/>
     </row>
-    <row r="71" ht="15" customHeight="1">
+    <row r="71" ht="13.65" customHeight="1">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -5202,7 +5183,7 @@
       <c r="AB71" s="3"/>
       <c r="AC71" s="3"/>
     </row>
-    <row r="72" ht="15" customHeight="1">
+    <row r="72" ht="13.65" customHeight="1">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -5233,7 +5214,7 @@
       <c r="AB72" s="3"/>
       <c r="AC72" s="3"/>
     </row>
-    <row r="73" ht="15" customHeight="1">
+    <row r="73" ht="13.65" customHeight="1">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -5264,7 +5245,7 @@
       <c r="AB73" s="3"/>
       <c r="AC73" s="3"/>
     </row>
-    <row r="74" ht="15" customHeight="1">
+    <row r="74" ht="13.65" customHeight="1">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5295,7 +5276,7 @@
       <c r="AB74" s="3"/>
       <c r="AC74" s="3"/>
     </row>
-    <row r="75" ht="15" customHeight="1">
+    <row r="75" ht="13.65" customHeight="1">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5326,7 +5307,7 @@
       <c r="AB75" s="3"/>
       <c r="AC75" s="3"/>
     </row>
-    <row r="76" ht="15" customHeight="1">
+    <row r="76" ht="13.65" customHeight="1">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5357,7 +5338,7 @@
       <c r="AB76" s="3"/>
       <c r="AC76" s="3"/>
     </row>
-    <row r="77" ht="15" customHeight="1">
+    <row r="77" ht="13.65" customHeight="1">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5388,7 +5369,7 @@
       <c r="AB77" s="3"/>
       <c r="AC77" s="3"/>
     </row>
-    <row r="78" ht="15" customHeight="1">
+    <row r="78" ht="13.65" customHeight="1">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5419,7 +5400,7 @@
       <c r="AB78" s="3"/>
       <c r="AC78" s="3"/>
     </row>
-    <row r="79" ht="15" customHeight="1">
+    <row r="79" ht="13.65" customHeight="1">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5450,7 +5431,7 @@
       <c r="AB79" s="3"/>
       <c r="AC79" s="3"/>
     </row>
-    <row r="80" ht="15" customHeight="1">
+    <row r="80" ht="13.65" customHeight="1">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5481,7 +5462,7 @@
       <c r="AB80" s="3"/>
       <c r="AC80" s="3"/>
     </row>
-    <row r="81" ht="15" customHeight="1">
+    <row r="81" ht="13.65" customHeight="1">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5512,7 +5493,7 @@
       <c r="AB81" s="3"/>
       <c r="AC81" s="3"/>
     </row>
-    <row r="82" ht="15" customHeight="1">
+    <row r="82" ht="13.65" customHeight="1">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5543,7 +5524,7 @@
       <c r="AB82" s="3"/>
       <c r="AC82" s="3"/>
     </row>
-    <row r="83" ht="15" customHeight="1">
+    <row r="83" ht="13.65" customHeight="1">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5574,7 +5555,7 @@
       <c r="AB83" s="3"/>
       <c r="AC83" s="3"/>
     </row>
-    <row r="84" ht="15" customHeight="1">
+    <row r="84" ht="13.65" customHeight="1">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5605,7 +5586,7 @@
       <c r="AB84" s="3"/>
       <c r="AC84" s="3"/>
     </row>
-    <row r="85" ht="15" customHeight="1">
+    <row r="85" ht="13.65" customHeight="1">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5636,7 +5617,7 @@
       <c r="AB85" s="3"/>
       <c r="AC85" s="3"/>
     </row>
-    <row r="86" ht="15" customHeight="1">
+    <row r="86" ht="13.65" customHeight="1">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5667,7 +5648,7 @@
       <c r="AB86" s="3"/>
       <c r="AC86" s="3"/>
     </row>
-    <row r="87" ht="15" customHeight="1">
+    <row r="87" ht="13.65" customHeight="1">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5698,7 +5679,7 @@
       <c r="AB87" s="3"/>
       <c r="AC87" s="3"/>
     </row>
-    <row r="88" ht="15" customHeight="1">
+    <row r="88" ht="13.65" customHeight="1">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5729,7 +5710,7 @@
       <c r="AB88" s="3"/>
       <c r="AC88" s="3"/>
     </row>
-    <row r="89" ht="15" customHeight="1">
+    <row r="89" ht="13.65" customHeight="1">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5760,7 +5741,7 @@
       <c r="AB89" s="3"/>
       <c r="AC89" s="3"/>
     </row>
-    <row r="90" ht="15" customHeight="1">
+    <row r="90" ht="13.65" customHeight="1">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5791,7 +5772,7 @@
       <c r="AB90" s="3"/>
       <c r="AC90" s="3"/>
     </row>
-    <row r="91" ht="15" customHeight="1">
+    <row r="91" ht="13.65" customHeight="1">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5822,7 +5803,7 @@
       <c r="AB91" s="3"/>
       <c r="AC91" s="3"/>
     </row>
-    <row r="92" ht="15" customHeight="1">
+    <row r="92" ht="13.65" customHeight="1">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5853,7 +5834,7 @@
       <c r="AB92" s="3"/>
       <c r="AC92" s="3"/>
     </row>
-    <row r="93" ht="15" customHeight="1">
+    <row r="93" ht="13.65" customHeight="1">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5884,7 +5865,7 @@
       <c r="AB93" s="3"/>
       <c r="AC93" s="3"/>
     </row>
-    <row r="94" ht="15" customHeight="1">
+    <row r="94" ht="13.65" customHeight="1">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5915,7 +5896,7 @@
       <c r="AB94" s="3"/>
       <c r="AC94" s="3"/>
     </row>
-    <row r="95" ht="15" customHeight="1">
+    <row r="95" ht="13.65" customHeight="1">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5946,7 +5927,7 @@
       <c r="AB95" s="3"/>
       <c r="AC95" s="3"/>
     </row>
-    <row r="96" ht="15" customHeight="1">
+    <row r="96" ht="13.65" customHeight="1">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5977,7 +5958,7 @@
       <c r="AB96" s="3"/>
       <c r="AC96" s="3"/>
     </row>
-    <row r="97" ht="15" customHeight="1">
+    <row r="97" ht="13.65" customHeight="1">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -6008,7 +5989,7 @@
       <c r="AB97" s="3"/>
       <c r="AC97" s="3"/>
     </row>
-    <row r="98" ht="15" customHeight="1">
+    <row r="98" ht="13.65" customHeight="1">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -6039,7 +6020,7 @@
       <c r="AB98" s="3"/>
       <c r="AC98" s="3"/>
     </row>
-    <row r="99" ht="15" customHeight="1">
+    <row r="99" ht="13.65" customHeight="1">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -6070,7 +6051,7 @@
       <c r="AB99" s="3"/>
       <c r="AC99" s="3"/>
     </row>
-    <row r="100" ht="15" customHeight="1">
+    <row r="100" ht="13.65" customHeight="1">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -6101,7 +6082,7 @@
       <c r="AB100" s="3"/>
       <c r="AC100" s="3"/>
     </row>
-    <row r="101" ht="15" customHeight="1">
+    <row r="101" ht="13.65" customHeight="1">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -6132,7 +6113,7 @@
       <c r="AB101" s="3"/>
       <c r="AC101" s="3"/>
     </row>
-    <row r="102" ht="15" customHeight="1">
+    <row r="102" ht="13.65" customHeight="1">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -6163,7 +6144,7 @@
       <c r="AB102" s="3"/>
       <c r="AC102" s="3"/>
     </row>
-    <row r="103" ht="15" customHeight="1">
+    <row r="103" ht="13.65" customHeight="1">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -6194,7 +6175,7 @@
       <c r="AB103" s="3"/>
       <c r="AC103" s="3"/>
     </row>
-    <row r="104" ht="15" customHeight="1">
+    <row r="104" ht="13.65" customHeight="1">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -6225,7 +6206,7 @@
       <c r="AB104" s="3"/>
       <c r="AC104" s="3"/>
     </row>
-    <row r="105" ht="15" customHeight="1">
+    <row r="105" ht="13.65" customHeight="1">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -6256,7 +6237,7 @@
       <c r="AB105" s="3"/>
       <c r="AC105" s="3"/>
     </row>
-    <row r="106" ht="15" customHeight="1">
+    <row r="106" ht="13.65" customHeight="1">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -6287,7 +6268,7 @@
       <c r="AB106" s="3"/>
       <c r="AC106" s="3"/>
     </row>
-    <row r="107" ht="15" customHeight="1">
+    <row r="107" ht="13.65" customHeight="1">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -6318,7 +6299,7 @@
       <c r="AB107" s="3"/>
       <c r="AC107" s="3"/>
     </row>
-    <row r="108" ht="15" customHeight="1">
+    <row r="108" ht="13.65" customHeight="1">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -6349,7 +6330,7 @@
       <c r="AB108" s="3"/>
       <c r="AC108" s="3"/>
     </row>
-    <row r="109" ht="15" customHeight="1">
+    <row r="109" ht="13.65" customHeight="1">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -6380,7 +6361,7 @@
       <c r="AB109" s="3"/>
       <c r="AC109" s="3"/>
     </row>
-    <row r="110" ht="15" customHeight="1">
+    <row r="110" ht="13.65" customHeight="1">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -6411,7 +6392,7 @@
       <c r="AB110" s="3"/>
       <c r="AC110" s="3"/>
     </row>
-    <row r="111" ht="15" customHeight="1">
+    <row r="111" ht="13.65" customHeight="1">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -6442,7 +6423,7 @@
       <c r="AB111" s="3"/>
       <c r="AC111" s="3"/>
     </row>
-    <row r="112" ht="15" customHeight="1">
+    <row r="112" ht="13.65" customHeight="1">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -6473,7 +6454,7 @@
       <c r="AB112" s="3"/>
       <c r="AC112" s="3"/>
     </row>
-    <row r="113" ht="15" customHeight="1">
+    <row r="113" ht="13.65" customHeight="1">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6504,7 +6485,7 @@
       <c r="AB113" s="3"/>
       <c r="AC113" s="3"/>
     </row>
-    <row r="114" ht="15" customHeight="1">
+    <row r="114" ht="13.65" customHeight="1">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -6535,7 +6516,7 @@
       <c r="AB114" s="3"/>
       <c r="AC114" s="3"/>
     </row>
-    <row r="115" ht="15" customHeight="1">
+    <row r="115" ht="13.65" customHeight="1">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -6566,7 +6547,7 @@
       <c r="AB115" s="3"/>
       <c r="AC115" s="3"/>
     </row>
-    <row r="116" ht="15" customHeight="1">
+    <row r="116" ht="13.65" customHeight="1">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -6597,7 +6578,7 @@
       <c r="AB116" s="3"/>
       <c r="AC116" s="3"/>
     </row>
-    <row r="117" ht="15" customHeight="1">
+    <row r="117" ht="13.65" customHeight="1">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -6628,7 +6609,7 @@
       <c r="AB117" s="3"/>
       <c r="AC117" s="3"/>
     </row>
-    <row r="118" ht="15" customHeight="1">
+    <row r="118" ht="13.65" customHeight="1">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -6659,7 +6640,7 @@
       <c r="AB118" s="3"/>
       <c r="AC118" s="3"/>
     </row>
-    <row r="119" ht="15" customHeight="1">
+    <row r="119" ht="13.65" customHeight="1">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -6690,7 +6671,7 @@
       <c r="AB119" s="3"/>
       <c r="AC119" s="3"/>
     </row>
-    <row r="120" ht="15" customHeight="1">
+    <row r="120" ht="13.65" customHeight="1">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -6721,7 +6702,7 @@
       <c r="AB120" s="3"/>
       <c r="AC120" s="3"/>
     </row>
-    <row r="121" ht="15" customHeight="1">
+    <row r="121" ht="13.65" customHeight="1">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6752,7 +6733,7 @@
       <c r="AB121" s="3"/>
       <c r="AC121" s="3"/>
     </row>
-    <row r="122" ht="15" customHeight="1">
+    <row r="122" ht="13.65" customHeight="1">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -6783,7 +6764,7 @@
       <c r="AB122" s="3"/>
       <c r="AC122" s="3"/>
     </row>
-    <row r="123" ht="15" customHeight="1">
+    <row r="123" ht="13.65" customHeight="1">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -6814,7 +6795,7 @@
       <c r="AB123" s="3"/>
       <c r="AC123" s="3"/>
     </row>
-    <row r="124" ht="15" customHeight="1">
+    <row r="124" ht="13.65" customHeight="1">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -6845,7 +6826,7 @@
       <c r="AB124" s="3"/>
       <c r="AC124" s="3"/>
     </row>
-    <row r="125" ht="15" customHeight="1">
+    <row r="125" ht="13.65" customHeight="1">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6876,7 +6857,7 @@
       <c r="AB125" s="3"/>
       <c r="AC125" s="3"/>
     </row>
-    <row r="126" ht="15" customHeight="1">
+    <row r="126" ht="13.65" customHeight="1">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -6907,7 +6888,7 @@
       <c r="AB126" s="3"/>
       <c r="AC126" s="3"/>
     </row>
-    <row r="127" ht="15" customHeight="1">
+    <row r="127" ht="13.65" customHeight="1">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -6938,7 +6919,7 @@
       <c r="AB127" s="3"/>
       <c r="AC127" s="3"/>
     </row>
-    <row r="128" ht="15" customHeight="1">
+    <row r="128" ht="13.65" customHeight="1">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -6969,7 +6950,7 @@
       <c r="AB128" s="3"/>
       <c r="AC128" s="3"/>
     </row>
-    <row r="129" ht="15" customHeight="1">
+    <row r="129" ht="13.65" customHeight="1">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7000,7 +6981,7 @@
       <c r="AB129" s="3"/>
       <c r="AC129" s="3"/>
     </row>
-    <row r="130" ht="15" customHeight="1">
+    <row r="130" ht="13.65" customHeight="1">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -7031,7 +7012,7 @@
       <c r="AB130" s="3"/>
       <c r="AC130" s="3"/>
     </row>
-    <row r="131" ht="15" customHeight="1">
+    <row r="131" ht="13.65" customHeight="1">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -7062,7 +7043,7 @@
       <c r="AB131" s="3"/>
       <c r="AC131" s="3"/>
     </row>
-    <row r="132" ht="15" customHeight="1">
+    <row r="132" ht="13.65" customHeight="1">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -7093,7 +7074,7 @@
       <c r="AB132" s="3"/>
       <c r="AC132" s="3"/>
     </row>
-    <row r="133" ht="15" customHeight="1">
+    <row r="133" ht="13.65" customHeight="1">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -7124,7 +7105,7 @@
       <c r="AB133" s="3"/>
       <c r="AC133" s="3"/>
     </row>
-    <row r="134" ht="15" customHeight="1">
+    <row r="134" ht="13.65" customHeight="1">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -7155,7 +7136,7 @@
       <c r="AB134" s="3"/>
       <c r="AC134" s="3"/>
     </row>
-    <row r="135" ht="15" customHeight="1">
+    <row r="135" ht="13.65" customHeight="1">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -7186,7 +7167,7 @@
       <c r="AB135" s="3"/>
       <c r="AC135" s="3"/>
     </row>
-    <row r="136" ht="15" customHeight="1">
+    <row r="136" ht="13.65" customHeight="1">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -7217,7 +7198,7 @@
       <c r="AB136" s="3"/>
       <c r="AC136" s="3"/>
     </row>
-    <row r="137" ht="15" customHeight="1">
+    <row r="137" ht="13.65" customHeight="1">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -7248,7 +7229,7 @@
       <c r="AB137" s="3"/>
       <c r="AC137" s="3"/>
     </row>
-    <row r="138" ht="15" customHeight="1">
+    <row r="138" ht="13.65" customHeight="1">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -7279,7 +7260,7 @@
       <c r="AB138" s="3"/>
       <c r="AC138" s="3"/>
     </row>
-    <row r="139" ht="15" customHeight="1">
+    <row r="139" ht="13.65" customHeight="1">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -7310,7 +7291,7 @@
       <c r="AB139" s="3"/>
       <c r="AC139" s="3"/>
     </row>
-    <row r="140" ht="15" customHeight="1">
+    <row r="140" ht="13.65" customHeight="1">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -7341,7 +7322,7 @@
       <c r="AB140" s="3"/>
       <c r="AC140" s="3"/>
     </row>
-    <row r="141" ht="15" customHeight="1">
+    <row r="141" ht="13.65" customHeight="1">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -7372,7 +7353,7 @@
       <c r="AB141" s="3"/>
       <c r="AC141" s="3"/>
     </row>
-    <row r="142" ht="15" customHeight="1">
+    <row r="142" ht="13.65" customHeight="1">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -7403,7 +7384,7 @@
       <c r="AB142" s="3"/>
       <c r="AC142" s="3"/>
     </row>
-    <row r="143" ht="15" customHeight="1">
+    <row r="143" ht="13.65" customHeight="1">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -7434,7 +7415,7 @@
       <c r="AB143" s="3"/>
       <c r="AC143" s="3"/>
     </row>
-    <row r="144" ht="15" customHeight="1">
+    <row r="144" ht="13.65" customHeight="1">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -7465,7 +7446,7 @@
       <c r="AB144" s="3"/>
       <c r="AC144" s="3"/>
     </row>
-    <row r="145" ht="15" customHeight="1">
+    <row r="145" ht="13.65" customHeight="1">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -7496,7 +7477,7 @@
       <c r="AB145" s="3"/>
       <c r="AC145" s="3"/>
     </row>
-    <row r="146" ht="15" customHeight="1">
+    <row r="146" ht="13.65" customHeight="1">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -7527,7 +7508,7 @@
       <c r="AB146" s="3"/>
       <c r="AC146" s="3"/>
     </row>
-    <row r="147" ht="15" customHeight="1">
+    <row r="147" ht="13.65" customHeight="1">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -7558,7 +7539,7 @@
       <c r="AB147" s="3"/>
       <c r="AC147" s="3"/>
     </row>
-    <row r="148" ht="15" customHeight="1">
+    <row r="148" ht="13.65" customHeight="1">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -7589,7 +7570,7 @@
       <c r="AB148" s="3"/>
       <c r="AC148" s="3"/>
     </row>
-    <row r="149" ht="15" customHeight="1">
+    <row r="149" ht="13.65" customHeight="1">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -7620,7 +7601,7 @@
       <c r="AB149" s="3"/>
       <c r="AC149" s="3"/>
     </row>
-    <row r="150" ht="15" customHeight="1">
+    <row r="150" ht="13.65" customHeight="1">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -7651,7 +7632,7 @@
       <c r="AB150" s="3"/>
       <c r="AC150" s="3"/>
     </row>
-    <row r="151" ht="15" customHeight="1">
+    <row r="151" ht="13.65" customHeight="1">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -7682,7 +7663,7 @@
       <c r="AB151" s="3"/>
       <c r="AC151" s="3"/>
     </row>
-    <row r="152" ht="15" customHeight="1">
+    <row r="152" ht="13.65" customHeight="1">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -7713,7 +7694,7 @@
       <c r="AB152" s="3"/>
       <c r="AC152" s="3"/>
     </row>
-    <row r="153" ht="15" customHeight="1">
+    <row r="153" ht="13.65" customHeight="1">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -7744,7 +7725,7 @@
       <c r="AB153" s="3"/>
       <c r="AC153" s="3"/>
     </row>
-    <row r="154" ht="15" customHeight="1">
+    <row r="154" ht="13.65" customHeight="1">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -7775,7 +7756,7 @@
       <c r="AB154" s="3"/>
       <c r="AC154" s="3"/>
     </row>
-    <row r="155" ht="15" customHeight="1">
+    <row r="155" ht="13.65" customHeight="1">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -7806,7 +7787,7 @@
       <c r="AB155" s="3"/>
       <c r="AC155" s="3"/>
     </row>
-    <row r="156" ht="15" customHeight="1">
+    <row r="156" ht="13.65" customHeight="1">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -7837,7 +7818,7 @@
       <c r="AB156" s="3"/>
       <c r="AC156" s="3"/>
     </row>
-    <row r="157" ht="15" customHeight="1">
+    <row r="157" ht="13.65" customHeight="1">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -7868,7 +7849,7 @@
       <c r="AB157" s="3"/>
       <c r="AC157" s="3"/>
     </row>
-    <row r="158" ht="15" customHeight="1">
+    <row r="158" ht="13.65" customHeight="1">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -7899,7 +7880,7 @@
       <c r="AB158" s="3"/>
       <c r="AC158" s="3"/>
     </row>
-    <row r="159" ht="15" customHeight="1">
+    <row r="159" ht="13.65" customHeight="1">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -7931,7 +7912,7 @@
       <c r="AC159" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -7945,88 +7926,88 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.67188" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.67188" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.67188" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.67188" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.67188" style="4" customWidth="1"/>
     <col min="6" max="256" width="8.85156" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -8040,88 +8021,88 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="6" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.67188" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.67188" style="5" customWidth="1"/>
+    <col min="3" max="3" width="8.67188" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.67188" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.67188" style="5" customWidth="1"/>
+    <col min="6" max="256" width="8.85156" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>